<commit_message>
feat firts version 3.1
</commit_message>
<xml_diff>
--- a/unity_data/personajes/activos/Fëanor.xlsx
+++ b/unity_data/personajes/activos/Fëanor.xlsx
@@ -9,7 +9,6 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Estadisticas" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Info" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Roleplay" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -427,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,16 +445,6 @@
           <t>Valor</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Bonus_Items</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -464,13 +453,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3">
@@ -480,13 +463,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>8</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4">
@@ -496,13 +473,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>7</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5">
@@ -514,12 +485,6 @@
       <c r="B5" t="n">
         <v>7</v>
       </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>7</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -528,13 +493,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>6</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7">
@@ -544,13 +503,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>7</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
@@ -560,13 +513,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>5</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9">
@@ -576,13 +523,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>8</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="n">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -596,7 +537,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -643,151 +584,32 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Nivel</t>
+          <t>PV_Actual</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Experiencia</t>
+          <t>PV_Max</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>PV_Actual</t>
+          <t>Oro</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>PV_Max</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Oro</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Ubicación</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Desconocida</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Aspecto</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Contenido</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Descripción</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Trasfondo</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Personalidad</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Objetivos</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Miedos</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Aliados</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Enemigos</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>